<commit_message>
add multipanel plots for recoveries and non-baseline productivity MPSPs
</commit_message>
<xml_diff>
--- a/fermentation_insights/TRY_results/g_coeff_baselines_percentiles.xlsx
+++ b/fermentation_insights/TRY_results/g_coeff_baselines_percentiles.xlsx
@@ -699,13 +699,13 @@
         <v>0.6031912016243293</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6010186238550057</v>
+        <v>0.5986548995531681</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6014137107265549</v>
+        <v>0.5987440318041106</v>
       </c>
       <c r="G10" t="n">
-        <v>0.602043618437349</v>
+        <v>0.5988283263768763</v>
       </c>
     </row>
     <row r="11">
@@ -723,16 +723,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.6028488348905511</v>
+        <v>0.6028488348904371</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5878796681521615</v>
+        <v>0.5854047692975199</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5885187862166137</v>
+        <v>0.5857518754390745</v>
       </c>
       <c r="G11" t="n">
-        <v>0.5891170179878673</v>
+        <v>0.586100821567949</v>
       </c>
     </row>
     <row r="12">
@@ -750,16 +750,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.6027367034234429</v>
+        <v>0.6027367034234539</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5938542188089596</v>
+        <v>0.591779165550224</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5939109400288758</v>
+        <v>0.5923570483142888</v>
       </c>
       <c r="G12" t="n">
-        <v>0.5939638334198035</v>
+        <v>0.5924496053209782</v>
       </c>
     </row>
     <row r="13">
@@ -777,16 +777,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.6032564221695031</v>
+        <v>0.6032563360714954</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5954460434089589</v>
+        <v>0.5927185846790763</v>
       </c>
       <c r="F13" t="n">
-        <v>0.595763065016786</v>
+        <v>0.5928064600981822</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5960700468886163</v>
+        <v>0.5928909045560399</v>
       </c>
     </row>
     <row r="14">
@@ -807,13 +807,13 @@
         <v>0.626369466760216</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6239903717433044</v>
+        <v>0.6215865611896321</v>
       </c>
       <c r="F14" t="n">
-        <v>0.624632678099853</v>
+        <v>0.6216761342309467</v>
       </c>
       <c r="G14" t="n">
-        <v>0.62525646469042</v>
+        <v>0.6217654214631273</v>
       </c>
     </row>
     <row r="15">
@@ -831,16 +831,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.6258257611068714</v>
+        <v>0.625825761106789</v>
       </c>
       <c r="E15" t="n">
-        <v>0.6114213630217711</v>
+        <v>0.6088896977205107</v>
       </c>
       <c r="F15" t="n">
-        <v>0.612007871668953</v>
+        <v>0.6092256641852031</v>
       </c>
       <c r="G15" t="n">
-        <v>0.6126434268673036</v>
+        <v>0.6094382465732844</v>
       </c>
     </row>
     <row r="16">
@@ -858,16 +858,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.6258731801449157</v>
+        <v>0.6258731801449422</v>
       </c>
       <c r="E16" t="n">
-        <v>0.6164189239676208</v>
+        <v>0.6151550372018855</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6165417412970111</v>
+        <v>0.6157126652832703</v>
       </c>
       <c r="G16" t="n">
-        <v>0.6170759411149578</v>
+        <v>0.6158215982194363</v>
       </c>
     </row>
     <row r="17">
@@ -885,16 +885,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.6263624387182642</v>
+        <v>0.6263624387181024</v>
       </c>
       <c r="E17" t="n">
-        <v>0.6178782470182562</v>
+        <v>0.6160755651237659</v>
       </c>
       <c r="F17" t="n">
-        <v>0.6184949096173198</v>
+        <v>0.6161684793177287</v>
       </c>
       <c r="G17" t="n">
-        <v>0.6189489447565439</v>
+        <v>0.6162814775809038</v>
       </c>
     </row>
     <row r="18">

</xml_diff>